<commit_message>
Fix BOM: add display as separate item
</commit_message>
<xml_diff>
--- a/pcb/serial-logger-prototype.xlsx
+++ b/pcb/serial-logger-prototype.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="117">
   <si>
     <t xml:space="preserve">Sync</t>
   </si>
@@ -127,238 +128,250 @@
     <t xml:space="preserve">Jitter_Footprints:Molex_503480-1400-1x14-1MP_P0.5mm_Horizontal</t>
   </si>
   <si>
+    <t xml:space="preserve">503480-1400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3215747</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG/SWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector_PinHeader_1.27mm:PinHeader_2x05_P1.27mm_Vertical_SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTSH-105-01-L-DV-K-P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2856437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200-FTSH10501LDVKP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conn_01x04_Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector_PinSocket_2.54mm:PinSocket_1x04_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1593460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conn_01x04_Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector_PinHeader_2.54mm:PinHeader_1x04_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2888929</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J4,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conn_01x03_Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector_PinHeader_2.54mm:PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22µH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inductor_SMD:L_1812_4532Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LQH43PN220M26L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2219279</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2, R1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor_SMD:R_0402_1005Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7, R5, R13,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor_SMD:R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8, R6, R3, R4, R12,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9, R10,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotary_Encoder_Switch_DualLED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jitter_Footprints:PEL12D-4xxxS-Sxxxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEL12D-4225S-S2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-PEL12D4225SS2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW_SPDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jitter_Footprints:slide_switch_09.03201.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09.03201.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1608080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM32G070KBT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package_QFP:LQFP-32_7x7mm_P0.8mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3365394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-STM32G070KBT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74LVC3G17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package_SO:TSSOP-8_3x3mm_P0.65mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN74LVC3G17DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1236391</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLV70228_SOT23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLV70228DBVT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2492371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U4, U6,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sn74lv1t34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN74LV1T34DBVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3119564</t>
+  </si>
+  <si>
+    <t xml:space="preserve">595-SN74LV1T34DBVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLV61046ADB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLV61046ADBV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3007283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP1, TP2, TP5, TP6, TP7, TP8, TP9,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestPoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestPoint:TestPoint_Pad_D1.0mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP4, TP3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestPoint:TestPoint_Pad_D1.5mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display</t>
+  </si>
+  <si>
     <t xml:space="preserve">387-ELW2106AA</t>
   </si>
   <si>
-    <t xml:space="preserve">J1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JTAG/SWD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector_PinHeader_1.27mm:PinHeader_2x05_P1.27mm_Vertical_SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FTSH-105-01-L-DV-K-P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2856437</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200-FTSH10501LDVKP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J2,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conn_01x04_Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector_PinSocket_2.54mm:PinSocket_1x04_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1593460</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J3,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conn_01x04_Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector_PinHeader_2.54mm:PinHeader_1x04_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2888929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J4,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conn_01x03_Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector_PinHeader_2.54mm:PinHeader_1x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22µH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inductor_SMD:L_1812_4532Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LQH43PN220M26L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2219279</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2, R1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor_SMD:R_0402_1005Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7, R5, R13,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor_SMD:R_0603_1608Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8, R6, R3, R4, R12,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R9, R10,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R11,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R14,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotary_Encoder_Switch_DualLED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jitter_Footprints:PEL12D-4xxxS-Sxxxx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEL12D-4225S-S2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">652-PEL12D4225SS2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW2,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW_SPDT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jitter_Footprints:slide_switch_09.03201.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09.03201.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1608080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM32G070KBT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Package_QFP:LQFP-32_7x7mm_P0.8mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3365394</t>
-  </si>
-  <si>
-    <t xml:space="preserve">511-STM32G070KBT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74LVC3G17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Package_SO:TSSOP-8_3x3mm_P0.65mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SN74LVC3G17DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1236391</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U3,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TLV70228_SOT23-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TLV70228DBVT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2492371</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4, U6,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sn74lv1t34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SN74LV1T34DBVR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3119564</t>
-  </si>
-  <si>
-    <t xml:space="preserve">595-SN74LV1T34DBVR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U5,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TLV61046ADB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TLV61046ADBV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3007283</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP1, TP2, TP5, TP6, TP7, TP8, TP9,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestPoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestPoint:TestPoint_Pad_D1.0mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP4, TP3,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestPoint:TestPoint_Pad_D1.5mm</t>
+    <t xml:space="preserve">M2x14 (of M2x15, misschien zelfs x16?)</t>
   </si>
 </sst>
 </file>
@@ -408,7 +421,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,13 +431,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFADC5E7"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFCCE4"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFDFCCE4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF20000"/>
+        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
   </fills>
@@ -462,7 +487,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,11 +500,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -491,11 +516,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,7 +549,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFF20000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -533,7 +570,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDFCCE4"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -579,7 +616,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -636,14 +673,14 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="4" t="n">
@@ -651,8 +688,8 @@
         <v>2</v>
       </c>
       <c r="J2" s="5"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -679,7 +716,7 @@
       <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I3" s="4" t="n">
         <f aca="false">MAX(0,K$1*C3-J3)</f>
         <v>2</v>
       </c>
@@ -703,7 +740,7 @@
       <c r="G4" s="6" t="n">
         <v>2896350</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="I4" s="4" t="n">
         <f aca="false">MAX(0,K$1*C4-J4)</f>
         <v>10</v>
       </c>
@@ -727,7 +764,7 @@
       <c r="G5" s="6" t="n">
         <v>2611942</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="4" t="n">
         <f aca="false">MAX(0,K$1*C5-J5)</f>
         <v>16</v>
       </c>
@@ -776,7 +813,7 @@
       <c r="G7" s="6" t="n">
         <v>2470416</v>
       </c>
-      <c r="I7" s="1" t="n">
+      <c r="I7" s="4" t="n">
         <f aca="false">MAX(0,K$1*C7-J7)</f>
         <v>10</v>
       </c>
@@ -797,14 +834,13 @@
       <c r="E8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="1" t="s">
+      <c r="F8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="1" t="n">
+      <c r="G8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="4" t="n">
         <f aca="false">MAX(0,K$1*C8-J8)</f>
         <v>2</v>
       </c>
@@ -814,27 +850,27 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="I9" s="4" t="n">
         <f aca="false">MAX(0,K$1*C9-J9)</f>
         <v>2</v>
       </c>
@@ -844,21 +880,21 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="I10" s="4" t="n">
         <f aca="false">MAX(0,K$1*C10-J10)</f>
         <v>2</v>
       </c>
@@ -868,21 +904,21 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="I11" s="4" t="n">
         <f aca="false">MAX(0,K$1*C11-J11)</f>
         <v>2</v>
       </c>
@@ -892,16 +928,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G12" s="6"/>
       <c r="I12" s="1" t="n">
@@ -917,24 +953,24 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="I13" s="4" t="n">
         <f aca="false">MAX(0,K$1*C13-J13)</f>
         <v>2</v>
       </c>
@@ -944,21 +980,21 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G14" s="6" t="n">
         <v>2614287</v>
       </c>
-      <c r="I14" s="1" t="n">
+      <c r="I14" s="4" t="n">
         <f aca="false">MAX(0,K$1*C14-J14)</f>
         <v>4</v>
       </c>
@@ -968,21 +1004,21 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G15" s="6" t="n">
         <v>1469748</v>
       </c>
-      <c r="I15" s="1" t="n">
+      <c r="I15" s="4" t="n">
         <f aca="false">MAX(0,K$1*C15-J15)</f>
         <v>6</v>
       </c>
@@ -992,21 +1028,21 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G16" s="6" t="n">
         <v>1738864</v>
       </c>
-      <c r="I16" s="1" t="n">
+      <c r="I16" s="4" t="n">
         <f aca="false">MAX(0,K$1*C16-J16)</f>
         <v>10</v>
       </c>
@@ -1016,21 +1052,21 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G17" s="6" t="n">
         <v>9232605</v>
       </c>
-      <c r="I17" s="1" t="n">
+      <c r="I17" s="4" t="n">
         <f aca="false">MAX(0,K$1*C17-J17)</f>
         <v>4</v>
       </c>
@@ -1040,21 +1076,21 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G18" s="6" t="n">
         <v>2694532</v>
       </c>
-      <c r="I18" s="1" t="n">
+      <c r="I18" s="4" t="n">
         <f aca="false">MAX(0,K$1*C18-J18)</f>
         <v>2</v>
       </c>
@@ -1064,21 +1100,21 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>2447198</v>
       </c>
-      <c r="I19" s="1" t="n">
+      <c r="I19" s="4" t="n">
         <f aca="false">MAX(0,K$1*C19-J19)</f>
         <v>2</v>
       </c>
@@ -1088,25 +1124,25 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I20" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="I20" s="4" t="n">
         <f aca="false">MAX(0,K$1*C20-J20)</f>
         <v>2</v>
       </c>
@@ -1116,24 +1152,24 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I21" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="I21" s="4" t="n">
         <f aca="false">MAX(0,K$1*C21-J21)</f>
         <v>2</v>
       </c>
@@ -1143,27 +1179,27 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="G22" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I22" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="I22" s="4" t="n">
         <f aca="false">MAX(0,K$1*C22-J22)</f>
         <v>2</v>
       </c>
@@ -1173,24 +1209,24 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I23" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="I23" s="4" t="n">
         <f aca="false">MAX(0,K$1*C23-J23)</f>
         <v>2</v>
       </c>
@@ -1200,24 +1236,24 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="I24" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="I24" s="4" t="n">
         <f aca="false">MAX(0,K$1*C24-J24)</f>
         <v>2</v>
       </c>
@@ -1227,27 +1263,27 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I25" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="I25" s="4" t="n">
         <f aca="false">MAX(0,K$1*C25-J25)</f>
         <v>4</v>
       </c>
@@ -1257,24 +1293,24 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="I26" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="I26" s="4" t="n">
         <f aca="false">MAX(0,K$1*C26-J26)</f>
         <v>2</v>
       </c>
@@ -1300,90 +1336,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C30" s="7" t="s">
+    <row r="30" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="C30" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="D30" s="9" t="s">
         <v>110</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="G30" s="6"/>
       <c r="I30" s="1" t="n">
         <f aca="false">MAX(0,K$1*C30-J30)</f>
         <v>0</v>
       </c>
-      <c r="J30" s="8" t="n">
+      <c r="J30" s="10" t="n">
         <f aca="false">K$1*C30</f>
         <v>14</v>
       </c>
       <c r="K30" s="1"/>
       <c r="AMJ30" s="1"/>
     </row>
-    <row r="31" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="7" t="s">
+    <row r="31" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>112</v>
+      <c r="D31" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="G31" s="6"/>
       <c r="I31" s="1" t="n">
         <f aca="false">MAX(0,K$1*C31-J31)</f>
         <v>0</v>
       </c>
-      <c r="J31" s="8" t="n">
+      <c r="J31" s="10" t="n">
         <f aca="false">K$1*C31</f>
         <v>4</v>
       </c>
       <c r="AMJ31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G32" s="6"/>
       <c r="I32" s="1" t="n">
         <f aca="false">MAX(0,K$1*C32-J32)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G33" s="6"/>
       <c r="I33" s="1" t="n">
         <f aca="false">MAX(0,K$1*C33-J33)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="11"/>
+      <c r="C34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G34" s="6"/>
-      <c r="I34" s="1" t="n">
+      <c r="H34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I34" s="4" t="n">
         <f aca="false">MAX(0,K$1*C34-J34)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G35" s="6"/>
-      <c r="I35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="11"/>
+      <c r="C35" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G35" s="6" t="n">
+        <v>2494515</v>
+      </c>
+      <c r="I35" s="4" t="n">
         <f aca="false">MAX(0,K$1*C35-J35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1393,4 +1454,89 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="1" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>